<commit_message>
added dates to ganntt
</commit_message>
<xml_diff>
--- a/Proj plan:Ganntt /Thesis_Gannt_Feb2017.xlsx
+++ b/Proj plan:Ganntt /Thesis_Gannt_Feb2017.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Storage HD/Google Drive/IT Online/Thesis/From first thesis module/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Storage HD/Google Drive/IT Online/Thesis/Proj plan:Ganntt /"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Project Definition</t>
   </si>
@@ -78,12 +78,18 @@
   </si>
   <si>
     <t>Supervisor Checkin &amp; Feedback</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -101,7 +107,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,12 +132,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -152,12 +152,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -430,13 +441,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AY25"/>
+  <dimension ref="A1:AY26"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AD9" sqref="AD9"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="AB17" sqref="AB17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -444,9 +455,8 @@
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="19" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="28" width="2.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="51" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="51" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:51" x14ac:dyDescent="0.2">
@@ -459,333 +469,441 @@
     </row>
     <row r="2" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2">
-        <v>35</v>
-      </c>
-      <c r="C2">
-        <v>36</v>
-      </c>
-      <c r="D2">
-        <v>37</v>
-      </c>
-      <c r="E2">
-        <v>38</v>
-      </c>
-      <c r="F2">
-        <v>39</v>
-      </c>
-      <c r="G2">
-        <v>40</v>
-      </c>
-      <c r="H2">
-        <v>41</v>
-      </c>
-      <c r="I2">
-        <v>42</v>
-      </c>
-      <c r="J2">
-        <v>43</v>
-      </c>
-      <c r="K2">
-        <v>44</v>
-      </c>
-      <c r="L2">
-        <v>45</v>
-      </c>
-      <c r="M2">
-        <v>46</v>
-      </c>
-      <c r="N2">
-        <v>47</v>
-      </c>
-      <c r="O2">
-        <v>48</v>
-      </c>
-      <c r="P2">
-        <v>49</v>
-      </c>
-      <c r="Q2">
-        <v>50</v>
-      </c>
-      <c r="R2">
-        <v>51</v>
-      </c>
-      <c r="S2">
-        <v>52</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2">
-        <v>2</v>
-      </c>
-      <c r="V2">
-        <v>3</v>
-      </c>
-      <c r="W2">
-        <v>4</v>
-      </c>
-      <c r="X2">
-        <v>5</v>
-      </c>
-      <c r="Y2">
-        <v>6</v>
-      </c>
-      <c r="Z2">
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="T2" s="6">
+        <v>42737</v>
+      </c>
+      <c r="U2" s="6">
+        <v>42744</v>
+      </c>
+      <c r="V2" s="6">
+        <v>42751</v>
+      </c>
+      <c r="W2" s="6">
+        <v>42758</v>
+      </c>
+      <c r="X2" s="6">
+        <v>42765</v>
+      </c>
+      <c r="Y2" s="6">
+        <v>42772</v>
+      </c>
+      <c r="Z2" s="6">
+        <v>42779</v>
       </c>
       <c r="AA2" s="6">
-        <v>8</v>
-      </c>
-      <c r="AB2">
-        <v>9</v>
-      </c>
-      <c r="AC2">
-        <v>10</v>
-      </c>
-      <c r="AD2">
-        <v>11</v>
-      </c>
-      <c r="AE2">
-        <v>12</v>
-      </c>
-      <c r="AF2">
-        <v>13</v>
-      </c>
-      <c r="AG2">
-        <v>14</v>
-      </c>
-      <c r="AH2">
-        <v>15</v>
-      </c>
-      <c r="AI2">
-        <v>16</v>
-      </c>
-      <c r="AJ2">
-        <v>17</v>
-      </c>
-      <c r="AK2">
-        <v>18</v>
-      </c>
-      <c r="AL2">
-        <v>19</v>
-      </c>
-      <c r="AM2">
-        <v>20</v>
-      </c>
-      <c r="AN2">
-        <v>21</v>
-      </c>
-      <c r="AO2">
-        <v>22</v>
-      </c>
-      <c r="AP2">
-        <v>23</v>
-      </c>
-      <c r="AQ2">
-        <v>24</v>
-      </c>
-      <c r="AR2">
-        <v>25</v>
-      </c>
-      <c r="AS2">
-        <v>26</v>
-      </c>
-      <c r="AT2">
-        <v>27</v>
-      </c>
-      <c r="AU2">
-        <v>28</v>
-      </c>
-      <c r="AV2">
-        <v>29</v>
-      </c>
-      <c r="AW2">
-        <v>30</v>
-      </c>
-      <c r="AX2">
-        <v>31</v>
-      </c>
-      <c r="AY2">
-        <v>32</v>
+        <v>42786</v>
+      </c>
+      <c r="AB2" s="6">
+        <v>42793</v>
+      </c>
+      <c r="AC2" s="6">
+        <v>42800</v>
+      </c>
+      <c r="AD2" s="6">
+        <v>42807</v>
+      </c>
+      <c r="AE2" s="6">
+        <v>42814</v>
+      </c>
+      <c r="AF2" s="6">
+        <v>42821</v>
+      </c>
+      <c r="AG2" s="6">
+        <v>42828</v>
+      </c>
+      <c r="AH2" s="6">
+        <v>42835</v>
+      </c>
+      <c r="AI2" s="6">
+        <v>42842</v>
+      </c>
+      <c r="AJ2" s="6">
+        <v>42849</v>
+      </c>
+      <c r="AK2" s="6">
+        <v>42856</v>
+      </c>
+      <c r="AL2" s="6">
+        <v>42863</v>
+      </c>
+      <c r="AM2" s="6">
+        <v>42870</v>
+      </c>
+      <c r="AN2" s="6">
+        <v>42877</v>
+      </c>
+      <c r="AO2" s="6">
+        <v>42884</v>
+      </c>
+      <c r="AP2" s="6">
+        <v>42891</v>
+      </c>
+      <c r="AQ2" s="6">
+        <v>42898</v>
+      </c>
+      <c r="AR2" s="6">
+        <v>42905</v>
+      </c>
+      <c r="AS2" s="6">
+        <v>42912</v>
+      </c>
+      <c r="AT2" s="6">
+        <v>42919</v>
+      </c>
+      <c r="AU2" s="6">
+        <v>42926</v>
+      </c>
+      <c r="AV2" s="6">
+        <v>42933</v>
+      </c>
+      <c r="AW2" s="6">
+        <v>42940</v>
+      </c>
+      <c r="AX2" s="6">
+        <v>42947</v>
+      </c>
+      <c r="AY2" s="6">
+        <v>42954</v>
       </c>
     </row>
     <row r="3" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>35</v>
+      </c>
+      <c r="C3">
+        <v>36</v>
+      </c>
+      <c r="D3">
+        <v>37</v>
+      </c>
+      <c r="E3">
+        <v>38</v>
+      </c>
+      <c r="F3">
+        <v>39</v>
+      </c>
+      <c r="G3">
+        <v>40</v>
+      </c>
+      <c r="H3">
+        <v>41</v>
+      </c>
+      <c r="I3">
+        <v>42</v>
+      </c>
+      <c r="J3">
+        <v>43</v>
+      </c>
+      <c r="K3">
+        <v>44</v>
+      </c>
+      <c r="L3">
+        <v>45</v>
+      </c>
+      <c r="M3">
+        <v>46</v>
+      </c>
+      <c r="N3">
+        <v>47</v>
+      </c>
+      <c r="O3">
+        <v>48</v>
+      </c>
+      <c r="P3">
+        <v>49</v>
+      </c>
+      <c r="Q3">
+        <v>50</v>
+      </c>
+      <c r="R3">
+        <v>51</v>
+      </c>
+      <c r="S3">
+        <v>52</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>2</v>
+      </c>
+      <c r="V3">
+        <v>3</v>
+      </c>
+      <c r="W3">
+        <v>4</v>
+      </c>
+      <c r="X3">
+        <v>5</v>
+      </c>
+      <c r="Y3">
+        <v>6</v>
+      </c>
+      <c r="Z3">
+        <v>7</v>
+      </c>
+      <c r="AA3" s="5">
+        <v>8</v>
+      </c>
+      <c r="AB3">
+        <v>9</v>
+      </c>
+      <c r="AC3">
+        <v>10</v>
+      </c>
+      <c r="AD3">
+        <v>11</v>
+      </c>
+      <c r="AE3">
+        <v>12</v>
+      </c>
+      <c r="AF3">
+        <v>13</v>
+      </c>
+      <c r="AG3">
+        <v>14</v>
+      </c>
+      <c r="AH3">
+        <v>15</v>
+      </c>
+      <c r="AI3">
+        <v>16</v>
+      </c>
+      <c r="AJ3">
+        <v>17</v>
+      </c>
+      <c r="AK3">
+        <v>18</v>
+      </c>
+      <c r="AL3">
+        <v>19</v>
+      </c>
+      <c r="AM3">
+        <v>20</v>
+      </c>
+      <c r="AN3">
+        <v>21</v>
+      </c>
+      <c r="AO3">
+        <v>22</v>
+      </c>
+      <c r="AP3">
+        <v>23</v>
+      </c>
+      <c r="AQ3">
+        <v>24</v>
+      </c>
+      <c r="AR3">
+        <v>25</v>
+      </c>
+      <c r="AS3">
+        <v>26</v>
+      </c>
+      <c r="AT3">
+        <v>27</v>
+      </c>
+      <c r="AU3">
+        <v>28</v>
+      </c>
+      <c r="AV3">
+        <v>29</v>
+      </c>
+      <c r="AW3">
+        <v>30</v>
+      </c>
+      <c r="AX3">
+        <v>31</v>
+      </c>
+      <c r="AY3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
-      <c r="W7" s="4"/>
-      <c r="X7" s="4"/>
-      <c r="Y7" s="4"/>
-      <c r="Z7" s="4"/>
-      <c r="AA7" s="4"/>
-      <c r="AB7" s="3"/>
-      <c r="AC7" s="3"/>
     </row>
     <row r="8" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4"/>
+      <c r="AA8" s="4"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+    </row>
+    <row r="9" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="AD8" s="3"/>
-      <c r="AE8" s="3"/>
-      <c r="AF8" s="3"/>
-      <c r="AG8" s="3"/>
-    </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+      <c r="AF9" s="3"/>
+      <c r="AG9" s="3"/>
+    </row>
+    <row r="10" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="AF10" s="3"/>
-      <c r="AG10" s="3"/>
-      <c r="AH10" s="3"/>
-      <c r="AI10" s="3"/>
-      <c r="AJ10" s="3"/>
-      <c r="AK10" s="3"/>
     </row>
     <row r="11" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>8</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="AF11" s="3"/>
+      <c r="AG11" s="3"/>
+      <c r="AH11" s="3"/>
+      <c r="AI11" s="3"/>
       <c r="AJ11" s="3"/>
       <c r="AK11" s="3"/>
-      <c r="AL11" s="3"/>
-      <c r="AM11" s="3"/>
-      <c r="AN11" s="3"/>
-      <c r="AO11" s="3"/>
-      <c r="AP11" s="3"/>
-      <c r="AQ11" s="3"/>
-      <c r="AR11" s="3"/>
-      <c r="AS11" s="3"/>
     </row>
     <row r="12" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ12" s="3"/>
+      <c r="AK12" s="3"/>
+      <c r="AL12" s="3"/>
+      <c r="AM12" s="3"/>
+      <c r="AN12" s="3"/>
+      <c r="AO12" s="3"/>
+      <c r="AP12" s="3"/>
+      <c r="AQ12" s="3"/>
+      <c r="AR12" s="3"/>
+      <c r="AS12" s="3"/>
+    </row>
+    <row r="13" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AT12" s="3"/>
-      <c r="AU12" s="3"/>
-      <c r="AV12" s="3"/>
-    </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="AT13" s="3"/>
+      <c r="AU13" s="3"/>
+      <c r="AV13" s="3"/>
+    </row>
+    <row r="14" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AP14" s="3"/>
-      <c r="AQ14" s="3"/>
-      <c r="AR14" s="3"/>
-      <c r="AS14" s="3"/>
-      <c r="AT14" s="3"/>
-      <c r="AU14" s="3"/>
-      <c r="AV14" s="3"/>
-      <c r="AW14" s="3"/>
     </row>
     <row r="15" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="AP15" s="3"/>
+      <c r="AQ15" s="3"/>
+      <c r="AR15" s="3"/>
+      <c r="AS15" s="3"/>
+      <c r="AT15" s="3"/>
+      <c r="AU15" s="3"/>
+      <c r="AV15" s="3"/>
       <c r="AW15" s="3"/>
-      <c r="AX15" s="3"/>
     </row>
     <row r="16" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW16" s="3"/>
+      <c r="AX16" s="3"/>
+    </row>
+    <row r="17" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AY16" s="3"/>
-    </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="AY17" s="3"/>
+    </row>
+    <row r="18" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="R17" s="5"/>
-      <c r="T17" s="4"/>
-      <c r="V17" s="4"/>
-      <c r="X17" s="4"/>
-      <c r="Z17" s="4"/>
-      <c r="AB17" s="3"/>
-      <c r="AD17" s="3"/>
-      <c r="AF17" s="3"/>
-      <c r="AH17" s="3"/>
-      <c r="AJ17" s="3"/>
-      <c r="AL17" s="3"/>
-      <c r="AN17" s="3"/>
-      <c r="AP17" s="3"/>
-      <c r="AR17" s="3"/>
-      <c r="AT17" s="3"/>
-      <c r="AV17" s="3"/>
-      <c r="AX17" s="3"/>
-    </row>
-    <row r="24" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="D18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="R18" s="5"/>
+      <c r="T18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="X18" s="4"/>
+      <c r="Z18" s="4"/>
+      <c r="AA18" s="4"/>
+      <c r="AB18" s="3"/>
+      <c r="AD18" s="3"/>
+      <c r="AF18" s="3"/>
+      <c r="AH18" s="3"/>
+      <c r="AJ18" s="3"/>
+      <c r="AL18" s="3"/>
+      <c r="AN18" s="3"/>
+      <c r="AP18" s="3"/>
+      <c r="AR18" s="3"/>
+      <c r="AT18" s="3"/>
+      <c r="AV18" s="3"/>
+      <c r="AX18" s="3"/>
+    </row>
+    <row r="25" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="4"/>
+      <c r="B26" s="4"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="T2:AY2">
+    <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(T2,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(T2,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>